<commit_message>
updated tables to include family
</commit_message>
<xml_diff>
--- a/pivot_merge2.xlsx
+++ b/pivot_merge2.xlsx
@@ -446,247 +446,247 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>! Not Identified to Species</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Aira caryophyllea</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Artemisia californica</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Avena barbata</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Avena fatua</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Baccharis pilularis</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Brachypodium distachyon</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Briza maxima</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Briza minor</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Bromus catharticus</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Bromus diandrus</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Bromus hordeaceus</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Bromus vulgaris</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Calystegia macrostegia</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Calystegia purpurata</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Carduus pycnocephalus</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Chlorogalum pomeridianum</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Cotoneaster pannosus</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Cynosurus echinatus</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Danthonia californica</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Dichondra donelliana</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Diplacus aurantiacus</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Elymus glaucus</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Festuca bromoides</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Festuca perennis</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Festuca temulenta</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Fragaria vesca</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Frangula californica</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Geranium dissectum</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Hordeum depressum</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Hypochaeris glabra</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Hypochaeris radicata</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Linum bienne</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Logfia gallica</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Lonicera hispidula</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Lysimachia arvensis</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Madia gracilis</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Madia sativa</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Plantago erecta</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Plantago lanceolata</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Pseudognaphalium californicum</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Rubus ursinus</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Rytidosperma penicillatum</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Sonchus oleraceus</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Stipa pulchra</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Stipa purpurata</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Toxicodendron diversilobum</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Toxicoscordion fremontii</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Vicia sativa</t>
-        </is>
-      </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>unknown!!!!!!!!</t>
         </is>
       </c>
     </row>
@@ -702,27 +702,29 @@
           <t>MGP_01_HWY, Spring_2020</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>34.07</v>
+      </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>0.64</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>1.27</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>3.18</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>28.34</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>3.82</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.32</v>
       </c>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
@@ -732,10 +734,10 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="n">
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="n">
         <v>1.59</v>
       </c>
-      <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
@@ -745,38 +747,36 @@
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="n">
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="n">
         <v>0.64</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AI2" t="n">
         <v>3.5</v>
       </c>
-      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="n">
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="n">
         <v>2.55</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AQ2" t="n">
         <v>10.51</v>
       </c>
-      <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="n">
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="n">
         <v>0.32</v>
       </c>
-      <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="inlineStr"/>
-      <c r="AZ2" t="n">
-        <v>1.27</v>
-      </c>
+      <c r="AZ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -792,87 +792,87 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
         <v>9.720000000000001</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
         <v>3.24</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>54.17</v>
       </c>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="n">
         <v>0.46</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="n">
         <v>2.78</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>1.39</v>
       </c>
-      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="n">
         <v>4.17</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>0.93</v>
       </c>
-      <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AI3" t="inlineStr"/>
       <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
         <v>0.46</v>
       </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="n">
         <v>0.46</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
+      <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" t="n">
         <v>5.09</v>
       </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
       <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="n">
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="n">
         <v>0.46</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="AV3" t="n">
         <v>6.02</v>
       </c>
-      <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -886,81 +886,81 @@
           <t>MGP_01_HWY, Spring_2022</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>1.08</v>
+      </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
         <v>9.73</v>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
         <v>0.54</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>64.86</v>
       </c>
-      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="n">
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="n">
         <v>2.7</v>
       </c>
-      <c r="W4" t="n">
+      <c r="X4" t="n">
         <v>0.54</v>
       </c>
-      <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="n">
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="n">
         <v>1.08</v>
       </c>
-      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="n">
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="n">
         <v>0.54</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="n">
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="n">
         <v>4.86</v>
       </c>
-      <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="n">
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="n">
         <v>3.24</v>
       </c>
-      <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="inlineStr"/>
       <c r="AX4" t="inlineStr"/>
       <c r="AY4" t="inlineStr"/>
-      <c r="AZ4" t="n">
-        <v>1.08</v>
-      </c>
+      <c r="AZ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -974,19 +974,21 @@
           <t>MGP_02_OLH, Spring_2020</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>6.78</v>
+      </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
         <v>2.26</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>5.88</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>52.94</v>
       </c>
-      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -994,65 +996,63 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" t="n">
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="n">
         <v>4.07</v>
       </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" t="inlineStr"/>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
       <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="n">
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="n">
         <v>2.71</v>
       </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="inlineStr"/>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
       <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
       <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="inlineStr"/>
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="n">
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="n">
         <v>0.45</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="n">
-        <v>0</v>
-      </c>
+      <c r="AO5" t="inlineStr"/>
       <c r="AP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="n">
         <v>6.79</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AR5" t="n">
         <v>0.9</v>
       </c>
-      <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="n">
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="n">
         <v>4.52</v>
       </c>
-      <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
       <c r="AX5" t="inlineStr"/>
       <c r="AY5" t="inlineStr"/>
-      <c r="AZ5" t="n">
-        <v>2.26</v>
-      </c>
+      <c r="AZ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1066,23 +1066,25 @@
           <t>MGP_02_OLH, Spring_2021</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
         <v>19.23</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="n">
         <v>32.69</v>
       </c>
-      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="n">
         <v>0.77</v>
       </c>
-      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
@@ -1091,20 +1093,20 @@
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" t="n">
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="n">
         <v>2.69</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Y6" t="n">
         <v>2.31</v>
       </c>
-      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="n">
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="n">
         <v>0.77</v>
       </c>
-      <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
@@ -1112,32 +1114,30 @@
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="n">
+        <v>0</v>
+      </c>
       <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="n">
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="n">
         <v>13.85</v>
       </c>
-      <c r="AP6" t="n">
+      <c r="AQ6" t="n">
         <v>1.92</v>
       </c>
-      <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="n">
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="n">
         <v>5.38</v>
       </c>
-      <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="inlineStr"/>
-      <c r="AY6" t="n">
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="n">
         <v>0.38</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1152,24 +1152,26 @@
           <t>MGP_02_OLH, Spring_2022</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
         <v>0.41</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
         <v>10.7</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>32.92</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>18.11</v>
       </c>
-      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
@@ -1181,56 +1183,54 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="n">
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="n">
         <v>0.82</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Y7" t="n">
         <v>2.88</v>
       </c>
-      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="n">
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="n">
         <v>0.41</v>
       </c>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="n">
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="n">
         <v>2.06</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="n">
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="n">
         <v>12.35</v>
       </c>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="n">
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="n">
         <v>1.23</v>
       </c>
-      <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="n">
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="n">
         <v>7</v>
       </c>
-      <c r="AV7" t="n">
+      <c r="AW7" t="n">
         <v>1.23</v>
       </c>
-      <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="inlineStr"/>
       <c r="AY7" t="inlineStr"/>
-      <c r="AZ7" t="n">
-        <v>2.06</v>
-      </c>
+      <c r="AZ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1244,25 +1244,27 @@
           <t>MGP_03_POL, Spring_2020</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>7.640000000000001</v>
+      </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
         <v>2.14</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
         <v>21.41</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>22.32</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>21.71</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0.92</v>
       </c>
-      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -1271,56 +1273,54 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
         <v>0.61</v>
       </c>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="n">
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="n">
         <v>2.14</v>
       </c>
-      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="n">
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="n">
         <v>0.31</v>
       </c>
-      <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="n">
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="n">
         <v>0.31</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="inlineStr"/>
       <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="n">
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="n">
         <v>10.7</v>
       </c>
-      <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="n">
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="n">
         <v>4.28</v>
       </c>
-      <c r="AV8" t="inlineStr"/>
       <c r="AW8" t="inlineStr"/>
       <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="inlineStr"/>
-      <c r="AZ8" t="n">
-        <v>0.61</v>
-      </c>
+      <c r="AZ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1335,99 +1335,99 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
+        <v>8.779999999999999</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
         <v>4.96</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
         <v>6.11</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>21.37</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>3.82</v>
       </c>
-      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="n">
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
         <v>0.76</v>
       </c>
-      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="n">
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
         <v>0.38</v>
       </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="n">
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="n">
         <v>5.34</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>1.15</v>
       </c>
-      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="n">
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="n">
         <v>1.91</v>
       </c>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
       <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="n">
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="n">
         <v>1.15</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AJ9" t="n">
         <v>1.91</v>
       </c>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="n">
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="n">
         <v>5.34</v>
       </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" t="inlineStr"/>
+      <c r="AM9" t="n">
+        <v>0</v>
+      </c>
       <c r="AN9" t="inlineStr"/>
       <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="n">
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="n">
         <v>7.25</v>
       </c>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="n">
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="n">
         <v>2.67</v>
       </c>
-      <c r="AS9" t="n">
+      <c r="AT9" t="n">
         <v>10.69</v>
       </c>
-      <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="n">
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="n">
         <v>6.11</v>
       </c>
-      <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
-      <c r="AX9" t="n">
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="n">
         <v>0.76</v>
       </c>
-      <c r="AY9" t="n">
+      <c r="AZ9" t="n">
         <v>0.38</v>
-      </c>
-      <c r="AZ9" t="n">
-        <v>8.779999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1442,97 +1442,97 @@
           <t>MGP_03_POL, Spring_2022</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>3.83</v>
+      </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
         <v>2.68</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
         <v>3.07</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>37.16</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.77</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
         <v>3.83</v>
       </c>
-      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
         <v>0.38</v>
       </c>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="n">
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="n">
         <v>2.3</v>
       </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="n">
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="n">
         <v>3.07</v>
       </c>
-      <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="n">
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="n">
         <v>1.92</v>
       </c>
-      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="n">
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="n">
         <v>0.38</v>
       </c>
-      <c r="AI10" t="n">
+      <c r="AJ10" t="n">
         <v>3.83</v>
       </c>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="n">
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="n">
         <v>4.98</v>
       </c>
-      <c r="AL10" t="n">
+      <c r="AM10" t="n">
         <v>0.38</v>
       </c>
-      <c r="AM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN10" t="inlineStr"/>
+      <c r="AN10" t="n">
+        <v>0</v>
+      </c>
       <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="n">
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="n">
         <v>11.11</v>
       </c>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="n">
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="n">
         <v>3.83</v>
       </c>
-      <c r="AS10" t="inlineStr"/>
       <c r="AT10" t="inlineStr"/>
-      <c r="AU10" t="n">
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="n">
         <v>6.51</v>
       </c>
-      <c r="AV10" t="inlineStr"/>
-      <c r="AW10" t="n">
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="n">
         <v>1.53</v>
       </c>
-      <c r="AX10" t="inlineStr"/>
       <c r="AY10" t="inlineStr"/>
-      <c r="AZ10" t="n">
-        <v>2.68</v>
-      </c>
+      <c r="AZ10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>